<commit_message>
fix literacy data set
</commit_message>
<xml_diff>
--- a/raw_data/literacy_rates2.xlsx
+++ b/raw_data/literacy_rates2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chacepaulson/Downloads/final_proj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chacepaulson/Downloads/final_proj/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="545">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -1659,6 +1659,9 @@
   </si>
   <si>
     <t>NOTE</t>
+  </si>
+  <si>
+    <t>total population: 82.8%</t>
   </si>
 </sst>
 </file>
@@ -1975,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3800,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>362</v>
+        <v>544</v>
       </c>
       <c r="D107" t="s">
         <v>180</v>

</xml_diff>